<commit_message>
functional and non-functional requirements added
</commit_message>
<xml_diff>
--- a/Week5. Errors' correction and logic DB/Assignment5.xlsx
+++ b/Week5. Errors' correction and logic DB/Assignment5.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>#</t>
   </si>
@@ -113,6 +113,18 @@
   </si>
   <si>
     <t>в 16:00 04.10.12 должны прислать</t>
+  </si>
+  <si>
+    <t>Просрочено на 00:55</t>
+  </si>
+  <si>
+    <t>Окончательно выполнено 04.10.15 0:00</t>
+  </si>
+  <si>
+    <t>Продлено до 04.10.15 16:00</t>
+  </si>
+  <si>
+    <t>Продлено до 04.10.15 22:00 согласно замечаниям Влада</t>
   </si>
 </sst>
 </file>
@@ -131,12 +143,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -151,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -160,6 +184,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -464,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,10 +503,11 @@
     <col min="4" max="4" width="97.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,8 +530,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -519,9 +546,15 @@
       <c r="E2" s="3">
         <v>42280.791666666664</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="F2" s="3">
+        <v>42280.75</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -536,9 +569,12 @@
       <c r="E3" s="3">
         <v>42278.916666666664</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="F3" s="3">
+        <v>42278.895833333336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -553,8 +589,17 @@
       <c r="E4" s="3">
         <v>42280.75</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" s="3">
+        <v>42280.788194444445</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -571,7 +616,7 @@
         <v>42280.75</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -588,8 +633,8 @@
         <v>42281.583333333336</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -604,9 +649,15 @@
       <c r="E7" s="3">
         <v>42280.833333333336</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="F7" s="3">
+        <v>42280.831944444442</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -622,8 +673,8 @@
         <v>42280.833333333336</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -638,8 +689,11 @@
       <c r="E9" s="3">
         <v>42281.645833333336</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="3">
+        <v>42280.798611111109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>

</xml_diff>